<commit_message>
Updated and tested all manuscript supplement files. They all execute correctly with the new code structure!
</commit_message>
<xml_diff>
--- a/Calibration/Testing_March2021/Testing_Liu_et_al_2005.xlsx
+++ b/Calibration/Testing_March2021/Testing_Liu_et_al_2005.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - University of Cambridge\!!!!!!PHD\Fissure8_MI_Work\MagmaSat\Testing_Compiled_FinalOnes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiacovin/Dropbox/Research/__Manuscripts in Progress/__VESIcal/__TheCode/VESIcal/Calibration/Testing_March2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1777F025-38A8-4491-8361-37E94504E86A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E42AC6-8AA7-5C45-B160-9BEC37C34272}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{96E931E8-05EA-409C-8C76-4F4BDEBA4436}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25180" windowHeight="21180" xr2:uid="{96E931E8-05EA-409C-8C76-4F4BDEBA4436}"/>
   </bookViews>
   <sheets>
     <sheet name="Test 1" sheetId="6" r:id="rId1"/>
@@ -586,16 +586,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888A4F77-8E72-4E2A-87DE-BB9121969237}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -646,7 +646,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -700,7 +700,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -754,7 +754,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -808,7 +808,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -862,7 +862,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -916,7 +916,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
@@ -970,7 +970,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>22</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>24</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>23</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>24</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>24</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>23</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>24</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>23</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>23</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>24</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>21</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>23</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>23</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>24</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>21</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>24</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>23</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>23</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>24</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>21</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>23</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>24</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>21</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>24</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>21</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>23</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>21</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>23</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>24</v>
       </c>
@@ -3757,9 +3757,9 @@
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4507,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>23</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>23</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>23</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>23</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>23</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>23</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>23</v>
       </c>
@@ -5211,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>23</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>23</v>
       </c>
@@ -5299,7 +5299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>23</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>23</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>23</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>23</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>23</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>23</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>23</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>23</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>23</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>23</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>23</v>
       </c>
@@ -5783,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>23</v>
       </c>
@@ -5827,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>23</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>23</v>
       </c>
@@ -5915,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>23</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>23</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>23</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>23</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>23</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>23</v>
       </c>
@@ -6179,7 +6179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>23</v>
       </c>
@@ -6223,7 +6223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>23</v>
       </c>
@@ -6276,13 +6276,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A699B4-A228-40B9-AA95-34CFA6D89472}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>31</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>32</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>33</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>35</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>36</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>37</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>38</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
         <v>39</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>40</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>41</v>
       </c>

</xml_diff>